<commit_message>
Prem | add missing reginal data in balasore
</commit_message>
<xml_diff>
--- a/micrograft/Balasore/data.xlsx
+++ b/micrograft/Balasore/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
   <si>
     <t>Route Code</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>ଭାୟା-ବାହାନଗା-ସେରଗଡ-ରେମୁଣା</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଈଶ୍ୱରପୁର - କଣ୍ଡାଗରାଡ଼ି - ଶ୍ୟାମସୁନ୍ଦରପୁର -ଡାଖିନାରସିଂହପୁର -</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1271,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1278,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1899,7 +1902,9 @@
       <c r="D36" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="30">
       <c r="A37" s="2" t="s">

</xml_diff>